<commit_message>
code setup for master
</commit_message>
<xml_diff>
--- a/com.pregopower1/src/main/resources/TestDatat.xlsx
+++ b/com.pregopower1/src/main/resources/TestDatat.xlsx
@@ -1,21 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\workspace\com.pregopower1\src\main\resources\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1C758CD1-98C3-4EC0-865A-A8D5471AF22B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{A9CDA022-3F63-494B-A746-BD15C5744DDD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="20790" windowHeight="11820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="testdata" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,12 +20,56 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+  <si>
+    <t>TestCases</t>
+  </si>
+  <si>
+    <t>Data1</t>
+  </si>
+  <si>
+    <t>Data2</t>
+  </si>
+  <si>
+    <t>Data3</t>
+  </si>
+  <si>
+    <t>rahul</t>
+  </si>
+  <si>
+    <t>dhiraj</t>
+  </si>
+  <si>
+    <t>mane</t>
+  </si>
+  <si>
+    <t>login</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -52,13 +92,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -337,12 +380,49 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="10.5703125" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" customWidth="1"/>
+    <col min="3" max="3" width="6" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>